<commit_message>
update unit for CIMR MS template
</commit_message>
<xml_diff>
--- a/templates/dataplant/CIMR/CIMR_-_Mass_spectrometry.xlsx
+++ b/templates/dataplant/CIMR/CIMR_-_Mass_spectrometry.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="168">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -329,6 +329,9 @@
     <t>Parameter [data acquisition rate]</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit </t>
+  </si>
+  <si>
     <t>Term Source REF (DPBO:0000162)</t>
   </si>
   <si>
@@ -356,7 +359,7 @@
     <t>Parameter [mass resolution]</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit </t>
+    <t xml:space="preserve">Unit  </t>
   </si>
   <si>
     <t>Term Source REF (MS:1000011)</t>
@@ -368,7 +371,7 @@
     <t>Parameter [observed mass accuracy]</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit  </t>
+    <t xml:space="preserve">Unit   </t>
   </si>
   <si>
     <t>Term Source REF (MS:4000072)</t>
@@ -479,7 +482,7 @@
     <t>Max Mustermann</t>
   </si>
   <si>
-    <t>10 scans per second</t>
+    <t>spectra per second</t>
   </si>
   <si>
     <t>100-1000</t>
@@ -568,8 +571,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BX2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:BX2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BY2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:BY2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -646,8 +649,9 @@
     <filterColumn colId="73" hiddenButton="1"/>
     <filterColumn colId="74" hiddenButton="1"/>
     <filterColumn colId="75" hiddenButton="1"/>
+    <filterColumn colId="76" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="76">
+  <tableColumns count="77">
     <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Parameter [MS sample resuspension]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (DPBO:0000044)" totalsRowFunction="none"/>
@@ -699,31 +703,32 @@
     <tableColumn id="49" name="Term Source REF (NCIT:C48036)" totalsRowFunction="none"/>
     <tableColumn id="50" name="Term Accession Number (NCIT:C48036)" totalsRowFunction="none"/>
     <tableColumn id="51" name="Parameter [data acquisition rate]" totalsRowFunction="none"/>
-    <tableColumn id="52" name="Term Source REF (DPBO:0000162)" totalsRowFunction="none"/>
-    <tableColumn id="53" name="Term Accession Number (DPBO:0000162)" totalsRowFunction="none"/>
-    <tableColumn id="54" name="Parameter [m/z acquisition range]" totalsRowFunction="none"/>
-    <tableColumn id="55" name="Term Source REF (MS:4000069)" totalsRowFunction="none"/>
-    <tableColumn id="56" name="Term Accession Number (MS:4000069)" totalsRowFunction="none"/>
-    <tableColumn id="57" name="Component [Calibrant role]" totalsRowFunction="none"/>
-    <tableColumn id="58" name="Term Source REF (CAO:000088)" totalsRowFunction="none"/>
-    <tableColumn id="59" name="Term Accession Number (CAO:000088)" totalsRowFunction="none"/>
-    <tableColumn id="60" name="Parameter [mass resolution]" totalsRowFunction="none"/>
-    <tableColumn id="61" name="Unit " totalsRowFunction="none"/>
-    <tableColumn id="62" name="Term Source REF (MS:1000011)" totalsRowFunction="none"/>
-    <tableColumn id="63" name="Term Accession Number (MS:1000011)" totalsRowFunction="none"/>
-    <tableColumn id="64" name="Parameter [observed mass accuracy]" totalsRowFunction="none"/>
-    <tableColumn id="65" name="Unit  " totalsRowFunction="none"/>
-    <tableColumn id="66" name="Term Source REF (MS:4000072)" totalsRowFunction="none"/>
-    <tableColumn id="67" name="Term Accession Number (MS:4000072)" totalsRowFunction="none"/>
-    <tableColumn id="68" name="Component [acquisition software]" totalsRowFunction="none"/>
-    <tableColumn id="69" name="Term Source REF (MS:1001455)" totalsRowFunction="none"/>
-    <tableColumn id="70" name="Term Accession Number (MS:1001455)" totalsRowFunction="none"/>
-    <tableColumn id="71" name="Parameter [mass spectrometer lock spray]" totalsRowFunction="none"/>
-    <tableColumn id="72" name="Term Source REF (DPBO:0000163)" totalsRowFunction="none"/>
-    <tableColumn id="73" name="Term Accession Number (DPBO:0000163)" totalsRowFunction="none"/>
-    <tableColumn id="74" name="Output [Data]" totalsRowFunction="none"/>
-    <tableColumn id="75" name="Data Format" totalsRowFunction="none"/>
-    <tableColumn id="76" name="Data Selector Format" totalsRowFunction="none"/>
+    <tableColumn id="52" name="Unit " totalsRowFunction="none"/>
+    <tableColumn id="53" name="Term Source REF (DPBO:0000162)" totalsRowFunction="none"/>
+    <tableColumn id="54" name="Term Accession Number (DPBO:0000162)" totalsRowFunction="none"/>
+    <tableColumn id="55" name="Parameter [m/z acquisition range]" totalsRowFunction="none"/>
+    <tableColumn id="56" name="Term Source REF (MS:4000069)" totalsRowFunction="none"/>
+    <tableColumn id="57" name="Term Accession Number (MS:4000069)" totalsRowFunction="none"/>
+    <tableColumn id="58" name="Component [Calibrant role]" totalsRowFunction="none"/>
+    <tableColumn id="59" name="Term Source REF (CAO:000088)" totalsRowFunction="none"/>
+    <tableColumn id="60" name="Term Accession Number (CAO:000088)" totalsRowFunction="none"/>
+    <tableColumn id="61" name="Parameter [mass resolution]" totalsRowFunction="none"/>
+    <tableColumn id="62" name="Unit  " totalsRowFunction="none"/>
+    <tableColumn id="63" name="Term Source REF (MS:1000011)" totalsRowFunction="none"/>
+    <tableColumn id="64" name="Term Accession Number (MS:1000011)" totalsRowFunction="none"/>
+    <tableColumn id="65" name="Parameter [observed mass accuracy]" totalsRowFunction="none"/>
+    <tableColumn id="66" name="Unit   " totalsRowFunction="none"/>
+    <tableColumn id="67" name="Term Source REF (MS:4000072)" totalsRowFunction="none"/>
+    <tableColumn id="68" name="Term Accession Number (MS:4000072)" totalsRowFunction="none"/>
+    <tableColumn id="69" name="Component [acquisition software]" totalsRowFunction="none"/>
+    <tableColumn id="70" name="Term Source REF (MS:1001455)" totalsRowFunction="none"/>
+    <tableColumn id="71" name="Term Accession Number (MS:1001455)" totalsRowFunction="none"/>
+    <tableColumn id="72" name="Parameter [mass spectrometer lock spray]" totalsRowFunction="none"/>
+    <tableColumn id="73" name="Term Source REF (DPBO:0000163)" totalsRowFunction="none"/>
+    <tableColumn id="74" name="Term Accession Number (DPBO:0000163)" totalsRowFunction="none"/>
+    <tableColumn id="75" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="76" name="Data Format" totalsRowFunction="none"/>
+    <tableColumn id="77" name="Data Selector Format" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1269,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BX2"/>
+  <dimension ref="A1:BY2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1501,184 +1506,187 @@
       <c r="BX1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="BY1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" t="s">
+        <v>145</v>
+      </c>
+      <c r="V2" t="s">
+        <v>131</v>
+      </c>
+      <c r="W2" t="s">
+        <v>131</v>
+      </c>
+      <c r="X2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY2" t="s">
         <v>136</v>
       </c>
-      <c r="J2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" t="s">
-        <v>138</v>
-      </c>
-      <c r="L2" t="s">
-        <v>139</v>
-      </c>
-      <c r="M2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>130</v>
-      </c>
-      <c r="R2" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" t="s">
-        <v>130</v>
-      </c>
-      <c r="T2" t="s">
-        <v>130</v>
-      </c>
-      <c r="U2" t="s">
-        <v>144</v>
-      </c>
-      <c r="V2" t="s">
-        <v>130</v>
-      </c>
-      <c r="W2" t="s">
-        <v>130</v>
-      </c>
-      <c r="X2" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>155</v>
-      </c>
       <c r="AZ2" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="BA2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BB2" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="BC2" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="BD2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BE2" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="BF2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BG2" t="s">
         <v>28</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>158</v>
       </c>
       <c r="BH2" t="s">
         <v>159</v>
@@ -1687,16 +1695,16 @@
         <v>160</v>
       </c>
       <c r="BJ2" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="BK2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="BL2" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="BM2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="BN2" t="s">
         <v>163</v>
@@ -1708,28 +1716,31 @@
         <v>165</v>
       </c>
       <c r="BQ2" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="BR2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BS2" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="BT2" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="BU2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BV2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BW2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BX2" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>